<commit_message>
Adding ColorFormate action to the package
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/Concatenation/output5.xlsx
+++ b/src/test/resources/test_files/Concatenation/output5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Documents/ExcelColumnConvert/ExcelColumnConvert/src/test/resources/test_files/Concatenation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_1E1A45A959F66FFC05FC9890E2FCDA74EA589DD0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAF8992C-B4BC-4D0B-8CE2-0DE15E78B513}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_1E1A45A959F66FFC05FC9890E2FCDA74EA589DD0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61AD2408-2857-4912-8238-07A17F42599B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -81,6 +82,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,7 +378,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +423,7 @@
       <c r="B4">
         <v>40</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>400</v>
       </c>
     </row>

</xml_diff>